<commit_message>
added most enzymes, TODO: implement negative LiN sums
</commit_message>
<xml_diff>
--- a/enzyme initialization data.xlsx
+++ b/enzyme initialization data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -76,13 +76,22 @@
     <t xml:space="preserve">dpapAbundance</t>
   </si>
   <si>
+    <t xml:space="preserve">Heme Detoxification Protein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PF14_0446</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apAbundance</t>
+  </si>
+  <si>
     <t xml:space="preserve">HAP, Falcipain III</t>
   </si>
   <si>
     <t xml:space="preserve">PF11_0161</t>
   </si>
   <si>
-    <t xml:space="preserve">apAbundance</t>
+    <t xml:space="preserve">hdpAbundance</t>
   </si>
   <si>
     <t xml:space="preserve">Falcilysin</t>
@@ -91,19 +100,19 @@
     <t xml:space="preserve">PF13_0322</t>
   </si>
   <si>
+    <t xml:space="preserve">Aminoacyl proline aminopeptidase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pH</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dipeptidyl aminopeptidase</t>
   </si>
   <si>
-    <t xml:space="preserve">Aminoacyl proline aminopeptidase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pH</t>
+    <t xml:space="preserve">kcat/km</t>
   </si>
   <si>
     <t xml:space="preserve">Leucyl aminopeptidase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kcat/km</t>
   </si>
   <si>
     <t xml:space="preserve">Aspartyl aminopeptidase</t>
@@ -131,11 +140,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -157,6 +167,14 @@
       <color rgb="FF6A8759"/>
       <name val="DejaVu Sans Mono"/>
       <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF6A8759"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -201,12 +219,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -287,15 +309,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -442,23 +464,23 @@
       <c r="A6" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="0" t="n">
         <f aca="false">E6*10^3</f>
-        <v>148000</v>
+        <v>4179000</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">F6*10^(-6)</f>
-        <v>8E-005</v>
+        <v>5E-005</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>148</v>
+        <v>4179</v>
       </c>
       <c r="F6" s="0" t="n">
-        <f aca="false">$I$3</f>
-        <v>80</v>
+        <f aca="false">I7</f>
+        <v>50</v>
       </c>
       <c r="H6" s="0" t="s">
         <v>20</v>
@@ -471,7 +493,7 @@
       <c r="A7" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="0" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="0" t="n">
@@ -486,64 +508,73 @@
         <v>148</v>
       </c>
       <c r="F7" s="0" t="n">
-        <f aca="false">I4</f>
-        <v>80</v>
+        <f aca="false">$I$3</f>
+        <v>80</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C8" s="0" t="n">
         <f aca="false">E8*10^3</f>
-        <v>70000</v>
+        <v>148000</v>
       </c>
       <c r="D8" s="0" t="n">
         <f aca="false">F8*10^(-6)</f>
+        <v>8E-005</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>148</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <f aca="false">I4</f>
+        <v>80</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="0" t="n">
+        <f aca="false">E9*10^3</f>
+        <v>70000</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <f aca="false">F9*10^(-6)</f>
         <v>0.0001</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E9" s="0" t="n">
         <v>70</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F9" s="0" t="n">
         <f aca="false">I5</f>
         <v>100</v>
       </c>
-      <c r="H8" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="K8" s="0" t="n">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <f aca="false">E9*10^3</f>
-        <v>1500</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <f aca="false">F9*10^(-6)</f>
-        <v>8E-005</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <f aca="false">$I$6</f>
-        <v>80</v>
-      </c>
       <c r="I9" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J9" s="0" t="n">
         <f aca="false">16/0.14</f>
@@ -556,7 +587,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C10" s="0" t="n">
         <f aca="false">E10*10^3</f>
@@ -576,7 +607,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C11" s="0" t="n">
         <f aca="false">E11*10^3</f>
@@ -596,41 +627,41 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="1"/>
+        <v>32</v>
+      </c>
       <c r="C12" s="0" t="n">
         <f aca="false">E12*10^3</f>
-        <v>69000</v>
+        <v>1500</v>
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">F12*10^(-6)</f>
         <v>8E-005</v>
       </c>
       <c r="E12" s="0" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <f aca="false">$I$6</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="0" t="n">
+        <f aca="false">E13*10^3</f>
+        <v>69000</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <f aca="false">F13*10^(-6)</f>
+        <v>8E-005</v>
+      </c>
+      <c r="E13" s="0" t="n">
         <f aca="false">ROUNDDOWN(AVERAGE(J9:K9),0)</f>
         <v>69</v>
       </c>
-      <c r="F12" s="0" t="n">
-        <f aca="false">$I$6</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="0" t="n">
-        <f aca="false">E13*10^3</f>
-        <v>22000</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <f aca="false">F13*10^(-6)</f>
-        <v>8E-005</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <v>22</v>
-      </c>
       <c r="F13" s="0" t="n">
         <f aca="false">$I$6</f>
         <v>80</v>
@@ -638,18 +669,18 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C14" s="0" t="n">
         <f aca="false">E14*10^3</f>
-        <v>109000</v>
+        <v>22000</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">F14*10^(-6)</f>
         <v>8E-005</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>109</v>
+        <v>22</v>
       </c>
       <c r="F14" s="0" t="n">
         <f aca="false">$I$6</f>
@@ -658,20 +689,40 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C15" s="0" t="n">
         <f aca="false">E15*10^3</f>
-        <v>440000</v>
+        <v>109000</v>
       </c>
       <c r="D15" s="0" t="n">
         <f aca="false">F15*10^(-6)</f>
         <v>8E-005</v>
       </c>
       <c r="E15" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <f aca="false">$I$6</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <f aca="false">E16*10^3</f>
+        <v>440000</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <f aca="false">F16*10^(-6)</f>
+        <v>8E-005</v>
+      </c>
+      <c r="E16" s="0" t="n">
         <v>440</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F16" s="0" t="n">
         <f aca="false">$I$6</f>
         <v>80</v>
       </c>

</xml_diff>

<commit_message>
hdp added to enzyme list
</commit_message>
<xml_diff>
--- a/enzyme initialization data.xlsx
+++ b/enzyme initialization data.xlsx
@@ -312,13 +312,10 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>

<commit_message>
corrected enzyme init data, added rest of enzymes
</commit_message>
<xml_diff>
--- a/enzyme initialization data.xlsx
+++ b/enzyme initialization data.xlsx
@@ -219,8 +219,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -312,414 +316,417 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <f aca="false">E2*10^3</f>
         <v>600000</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <f aca="false">F2*10^(-6)</f>
         <v>3E-005</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>600</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <f aca="false">$I$2</f>
         <v>30</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="I2" s="1" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <f aca="false">E3*10^3</f>
         <v>500000</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <f aca="false">F3*10^(-6)</f>
         <v>3E-005</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <f aca="false">$I$2</f>
         <v>30</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="I3" s="1" t="n">
         <v>80</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <f aca="false">E4*10^3</f>
         <v>750000</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <f aca="false">F4*10^(-6)</f>
         <v>3E-005</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <f aca="false">15/0.02</f>
         <v>750</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="1" t="n">
         <f aca="false">$I$2</f>
         <v>30</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="H4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="I4" s="1" t="n">
         <v>80</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <f aca="false">E5*10^3</f>
         <v>1511000</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <f aca="false">F5*10^(-6)</f>
         <v>8E-005</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>1511</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <f aca="false">$I$3</f>
         <v>80</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="H5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="I5" s="1" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <f aca="false">E6*10^3</f>
         <v>4179000</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <f aca="false">F6*10^(-6)</f>
         <v>5E-005</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>4179</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="1" t="n">
         <f aca="false">I7</f>
         <v>50</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="H6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="0" t="n">
+      <c r="I6" s="1" t="n">
         <v>80</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <f aca="false">E7*10^3</f>
         <v>148000</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <f aca="false">F7*10^(-6)</f>
         <v>8E-005</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>148</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="1" t="n">
         <f aca="false">$I$3</f>
         <v>80</v>
       </c>
-      <c r="H7" s="0" t="s">
+      <c r="H7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="I7" s="1" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <f aca="false">E8*10^3</f>
         <v>148000</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <f aca="false">F8*10^(-6)</f>
         <v>8E-005</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>148</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="1" t="n">
         <f aca="false">I4</f>
         <v>80</v>
       </c>
-      <c r="H8" s="0" t="s">
+      <c r="H8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="I8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="0" t="n">
+      <c r="J8" s="1" t="n">
         <v>7.5</v>
       </c>
-      <c r="K8" s="0" t="n">
+      <c r="K8" s="1" t="n">
         <v>5.5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="0" t="n">
+      <c r="B9" s="2"/>
+      <c r="C9" s="1" t="n">
         <f aca="false">E9*10^3</f>
         <v>70000</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <f aca="false">F9*10^(-6)</f>
         <v>0.0001</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="1" t="n">
         <f aca="false">I5</f>
         <v>100</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="I9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J9" s="0" t="n">
+      <c r="J9" s="1" t="n">
         <f aca="false">16/0.14</f>
         <v>114.285714285714</v>
       </c>
-      <c r="K9" s="0" t="n">
+      <c r="K9" s="1" t="n">
         <f aca="false">160/6.7</f>
         <v>23.8805970149254</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <f aca="false">E10*10^3</f>
-        <v>1500</v>
-      </c>
-      <c r="D10" s="0" t="n">
+        <v>3200</v>
+      </c>
+      <c r="D10" s="1" t="n">
         <f aca="false">F10*10^(-6)</f>
         <v>8E-005</v>
       </c>
-      <c r="E10" s="0" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="F10" s="0" t="n">
+      <c r="E10" s="1" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="F10" s="1" t="n">
         <f aca="false">$I$6</f>
         <v>80</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <f aca="false">E11*10^3</f>
-        <v>1500</v>
-      </c>
-      <c r="D11" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="D11" s="1" t="n">
         <f aca="false">F11*10^(-6)</f>
         <v>8E-005</v>
       </c>
-      <c r="E11" s="0" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="F11" s="0" t="n">
+      <c r="E11" s="1" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F11" s="1" t="n">
         <f aca="false">$I$6</f>
         <v>80</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <f aca="false">E12*10^3</f>
-        <v>1500</v>
-      </c>
-      <c r="D12" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="D12" s="1" t="n">
         <f aca="false">F12*10^(-6)</f>
         <v>8E-005</v>
       </c>
-      <c r="E12" s="0" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="F12" s="0" t="n">
+      <c r="E12" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="F12" s="1" t="n">
         <f aca="false">$I$6</f>
         <v>80</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="0" t="n">
+      <c r="B13" s="2"/>
+      <c r="C13" s="1" t="n">
         <f aca="false">E13*10^3</f>
         <v>69000</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <f aca="false">F13*10^(-6)</f>
         <v>8E-005</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <f aca="false">ROUNDDOWN(AVERAGE(J9:K9),0)</f>
         <v>69</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13" s="1" t="n">
         <f aca="false">$I$6</f>
         <v>80</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="1" t="n">
         <f aca="false">E14*10^3</f>
-        <v>22000</v>
-      </c>
-      <c r="D14" s="0" t="n">
+        <v>27400</v>
+      </c>
+      <c r="D14" s="1" t="n">
         <f aca="false">F14*10^(-6)</f>
         <v>8E-005</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="F14" s="0" t="n">
+        <v>27.4</v>
+      </c>
+      <c r="F14" s="1" t="n">
         <f aca="false">$I$6</f>
         <v>80</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <f aca="false">E15*10^3</f>
-        <v>109000</v>
-      </c>
-      <c r="D15" s="0" t="n">
+        <v>104000</v>
+      </c>
+      <c r="D15" s="1" t="n">
         <f aca="false">F15*10^(-6)</f>
         <v>8E-005</v>
       </c>
-      <c r="E15" s="0" t="n">
-        <v>109</v>
-      </c>
-      <c r="F15" s="0" t="n">
+      <c r="E15" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="F15" s="1" t="n">
         <f aca="false">$I$6</f>
         <v>80</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="1" t="n">
         <f aca="false">E16*10^3</f>
         <v>440000</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <f aca="false">F16*10^(-6)</f>
         <v>8E-005</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>440</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16" s="1" t="n">
         <f aca="false">$I$6</f>
         <v>80</v>
       </c>

</xml_diff>